<commit_message>
added user input for capturing path
</commit_message>
<xml_diff>
--- a/batchfile/qa_check_report.xlsx
+++ b/batchfile/qa_check_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>fileid</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>qa_check2</t>
+  </si>
+  <si>
+    <t>qa_check3</t>
   </si>
   <si>
     <t>file_1.wav</t>
@@ -395,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,46 +414,58 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>